<commit_message>
add MIT License and authors
</commit_message>
<xml_diff>
--- a/results/20250206/Nitrogen_Estimations.xlsx
+++ b/results/20250206/Nitrogen_Estimations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\minstrel\kinetika\project_demetra\results\20250206\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56E014E4-1F96-4C49-B726-41CF043EEFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A62FB96-2F55-43A5-A1D8-8D19F5871431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{DA2565EB-2DBB-4544-ABEE-7884703BBC10}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>Nitrit</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>USD/kg</t>
+  </si>
+  <si>
+    <t>Current result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaber Bosch </t>
+  </si>
+  <si>
+    <t>USD/kg N</t>
   </si>
 </sst>
 </file>
@@ -2857,7 +2869,7 @@
   <dimension ref="B2:AE76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,7 +2880,9 @@
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="11.85546875" style="1" customWidth="1"/>
-    <col min="13" max="26" width="9.140625" style="1"/>
+    <col min="13" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="9.140625" style="1"/>
     <col min="27" max="27" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.140625" style="9"/>
     <col min="29" max="29" width="9.140625" style="1"/>
@@ -2890,7 +2904,7 @@
     </row>
     <row r="3" spans="2:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1">
-        <v>110</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2902,7 +2916,7 @@
       </c>
       <c r="D4" s="1">
         <f>D3/5</f>
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3">
         <f>14/(14+16*2)</f>
@@ -2910,7 +2924,17 @@
       </c>
       <c r="F4" s="4">
         <f>E4*D4</f>
-        <v>6.6956521739130439</v>
+        <v>15.217391304347828</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="3">
+        <f>C17</f>
+        <v>0.90539682539682564</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2922,7 +2946,7 @@
       </c>
       <c r="D5" s="1">
         <f>D3*4/5</f>
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="E5" s="3">
         <f>14/(14+16*3)</f>
@@ -2930,7 +2954,17 @@
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>19.870967741935484</v>
+        <v>45.161290322580641</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V5" s="3" t="str">
+        <f>ROUND(0.4/0.46,2)&amp;" - "&amp;ROUND(0.6/0.46,2)</f>
+        <v>0.87 - 1.3</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="Z5" s="3"/>
       <c r="AA5" s="11"/>
@@ -2943,7 +2977,7 @@
       </c>
       <c r="F6" s="4">
         <f>F5+F4</f>
-        <v>26.566619915848527</v>
+        <v>60.378681626928469</v>
       </c>
       <c r="Z6" s="3"/>
       <c r="AA6" s="11"/>
@@ -2971,14 +3005,14 @@
       </c>
       <c r="C8" s="6">
         <f>(C7*F6)/1000</f>
-        <v>0.15939971949509119</v>
+        <v>0.36227208976157077</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1">
         <f>C8*6*1000</f>
-        <v>956.39831697054706</v>
+        <v>2173.6325385694245</v>
       </c>
       <c r="Z8" s="3"/>
       <c r="AA8" s="11"/>
@@ -3059,7 +3093,7 @@
       </c>
       <c r="C15" s="6">
         <f>C14/(C8/1000)</f>
-        <v>41.15440115440115</v>
+        <v>18.107936507936511</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -3087,7 +3121,10 @@
       </c>
       <c r="C17" s="3">
         <f>C15*C16</f>
-        <v>2.0577200577200574</v>
+        <v>0.90539682539682564</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E17" s="5"/>
       <c r="Z17" s="3"/>
@@ -3118,7 +3155,7 @@
       </c>
       <c r="C20" s="3">
         <f>(1440/C10)*C8/1000</f>
-        <v>7.6511865357643774E-2</v>
+        <v>0.17389060308555399</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -3131,7 +3168,7 @@
     <row r="21" spans="2:31" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="4">
         <f>C20*365</f>
-        <v>27.926830855539979</v>
+        <v>63.470070126227206</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>20</v>

</xml_diff>